<commit_message>
investigated which optimisation meathod is best
</commit_message>
<xml_diff>
--- a/compressed_sensing/metadata.xlsx
+++ b/compressed_sensing/metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{722437CE-C478-4F8E-8BC9-72EDBAD03AAB}"/>
+  <xr:revisionPtr revIDLastSave="310" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B4853EC-87A4-4A8D-AB4D-721FD9DF1778}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>array height (pixels)</t>
+  </si>
+  <si>
+    <t>1dmockanderrors11.csv</t>
+  </si>
+  <si>
+    <t>vibrations std (mm)</t>
+  </si>
+  <si>
+    <t>1dmockanderrors12.csv</t>
   </si>
 </sst>
 </file>
@@ -203,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -245,9 +254,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:L13" totalsRowShown="0">
-  <autoFilter ref="B3:L13" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M15" totalsRowShown="0">
+  <autoFilter ref="B3:M15" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
     <tableColumn id="3" xr3:uid="{8B3B76E6-8846-456D-9233-E504C5865E46}" name="pixel pitch (um)"/>
@@ -256,6 +265,7 @@
     <tableColumn id="6" xr3:uid="{F6FEC940-94A4-4334-A8FE-D49C7E756E64}" name="theta (arcminutes)"/>
     <tableColumn id="7" xr3:uid="{F5D180E3-248F-466D-95F2-4F2554B23077}" name="incoherance waves"/>
     <tableColumn id="8" xr3:uid="{334D7646-041A-4CD9-990E-A8353CC5883B}" name="incoherance std"/>
+    <tableColumn id="12" xr3:uid="{EEC5ECE7-5C4A-402F-9684-37843BF5E9E6}" name="vibrations std (mm)"/>
     <tableColumn id="9" xr3:uid="{7D0FA3B7-8FA7-420A-8CFE-F44A0DAE7D03}" name="read noise (% of coherant peak)"/>
     <tableColumn id="10" xr3:uid="{4AE8919A-F958-435F-ADCF-7F276B985BD9}" name="averages"/>
     <tableColumn id="11" xr3:uid="{3A0584E7-BBFA-4F43-8CB0-19FBDA7942D4}" name="Comments"/>
@@ -550,21 +560,21 @@
   <dimension ref="B1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -728,28 +738,28 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -764,29 +774,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:L13"/>
+  <dimension ref="B2:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -812,16 +823,19 @@
         <v>15</v>
       </c>
       <c r="J3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -847,16 +861,19 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>20</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -885,13 +902,16 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>20</v>
-      </c>
-      <c r="L5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>20</v>
+      </c>
+      <c r="M5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -920,13 +940,16 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>20</v>
-      </c>
-      <c r="L6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -952,16 +975,19 @@
         <v>1.6</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>20</v>
-      </c>
-      <c r="L7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -987,16 +1013,19 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>20</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -1022,16 +1051,19 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>20</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9">
+        <v>20</v>
+      </c>
+      <c r="M9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -1057,16 +1089,19 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>20</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10">
+        <v>20</v>
+      </c>
+      <c r="M10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -1092,16 +1127,19 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <v>20</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11">
+        <v>20</v>
+      </c>
+      <c r="M11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -1127,16 +1165,19 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <v>20</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12">
+        <v>20</v>
+      </c>
+      <c r="M12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>33</v>
       </c>
@@ -1162,18 +1203,91 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <v>20</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13">
+        <v>20</v>
+      </c>
+      <c r="M13" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>200</v>
+      </c>
+      <c r="D14">
+        <v>200</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>60</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+      <c r="L14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+      <c r="D15">
+        <v>200</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>60</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1193,18 +1307,18 @@
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
Created graphs for optimisation comparason presentation
</commit_message>
<xml_diff>
--- a/compressed_sensing/metadata.xlsx
+++ b/compressed_sensing/metadata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="310" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B4853EC-87A4-4A8D-AB4D-721FD9DF1778}"/>
+  <xr:revisionPtr revIDLastSave="367" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA83F140-DA21-492F-938A-095B257C5B9A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9615" yWindow="3570" windowWidth="28725" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
     <sheet name="1D NEW" sheetId="2" r:id="rId2"/>
-    <sheet name="2D" sheetId="3" r:id="rId3"/>
+    <sheet name="1D TRAINING" sheetId="4" r:id="rId3"/>
+    <sheet name="2D" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -167,6 +168,33 @@
   </si>
   <si>
     <t>1dmockanderrors12.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors13</t>
+  </si>
+  <si>
+    <t>training_set/</t>
+  </si>
+  <si>
+    <t>training_set1</t>
+  </si>
+  <si>
+    <t>training_set2</t>
+  </si>
+  <si>
+    <t>training_set3</t>
+  </si>
+  <si>
+    <t>0.1-10</t>
+  </si>
+  <si>
+    <t>0.1-3.16</t>
+  </si>
+  <si>
+    <t>number of interferograms</t>
+  </si>
+  <si>
+    <t>1dmockanderrors14</t>
   </si>
 </sst>
 </file>
@@ -210,9 +238,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -254,8 +285,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M15" totalsRowShown="0">
-  <autoFilter ref="B3:M15" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M17" totalsRowShown="0">
+  <autoFilter ref="B3:M17" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
@@ -275,6 +306,26 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{383F45E9-F2DB-40E5-BFB4-4F548F3A4AED}" name="Table432" displayName="Table432" ref="B3:L16" totalsRowShown="0">
+  <autoFilter ref="B3:L16" xr:uid="{383F45E9-F2DB-40E5-BFB4-4F548F3A4AED}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{40560E85-5A96-454C-824E-2802F027016B}" name="name"/>
+    <tableColumn id="2" xr3:uid="{0CBEA5B3-CEFE-4EF3-8016-FF4ED1C9B611}" name="array length (pixels)"/>
+    <tableColumn id="3" xr3:uid="{DEB5A3CB-BBAD-4FEE-853F-C1F23C44C720}" name="pixel pitch (um)"/>
+    <tableColumn id="4" xr3:uid="{CC161BE7-746F-44EF-8E18-A1269B000006}" name="central frequency (THz)"/>
+    <tableColumn id="5" xr3:uid="{5BBC0FEA-4269-40F2-A758-BA2ADF4F4385}" name="FWHM (THz)"/>
+    <tableColumn id="6" xr3:uid="{17843311-B1E8-417F-B5ED-17A99DB61355}" name="theta (arcminutes)"/>
+    <tableColumn id="12" xr3:uid="{1AA35316-E9AD-4DEC-A2E1-99878904A5AF}" name="vibrations std (mm)"/>
+    <tableColumn id="9" xr3:uid="{E08C02F2-548C-45E3-BFDF-B49F3484B5D7}" name="read noise (% of coherant peak)"/>
+    <tableColumn id="10" xr3:uid="{951BF258-4F23-4EE1-93C3-FC9E73ABA1C6}" name="averages"/>
+    <tableColumn id="7" xr3:uid="{616A40C2-F003-43D3-80B9-C3A9939AB34B}" name="number of interferograms"/>
+    <tableColumn id="11" xr3:uid="{63B18D46-6442-4333-BCA8-FEDBC2EA31FB}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2A5570FA-065E-4FD5-95DE-C8755D9E70C7}" name="Table426" displayName="Table426" ref="B3:L5" totalsRowShown="0">
   <autoFilter ref="B3:L5" xr:uid="{2A5570FA-065E-4FD5-95DE-C8755D9E70C7}"/>
   <tableColumns count="11">
@@ -566,15 +617,15 @@
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -774,28 +825,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:M15"/>
+  <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1282,6 +1333,76 @@
         <v>0</v>
       </c>
       <c r="L15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16">
+        <v>200</v>
+      </c>
+      <c r="D16">
+        <v>200</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>0.3</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>400</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>60</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+      <c r="L17">
         <v>30</v>
       </c>
     </row>
@@ -1297,6 +1418,172 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BFC62-FF4F-4DA1-97AB-A53A0749BD39}">
+  <dimension ref="B2:L6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5">
+        <v>60</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>30</v>
+      </c>
+      <c r="K5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>400</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6">
+        <v>60</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>30</v>
+      </c>
+      <c r="K6">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC75F5B-FD8B-46F1-B910-69CAC90BFB37}">
   <dimension ref="B2:L4"/>
   <sheetViews>
@@ -1307,18 +1594,18 @@
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
excel prevented last commit >:(
</commit_message>
<xml_diff>
--- a/compressed_sensing/metadata.xlsx
+++ b/compressed_sensing/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="367" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA83F140-DA21-492F-938A-095B257C5B9A}"/>
+  <xr:revisionPtr revIDLastSave="385" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{213011E1-DF3A-4728-9C14-03BF39FF574F}"/>
   <bookViews>
-    <workbookView xWindow="9615" yWindow="3570" windowWidth="28725" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>1dmockanderrors14</t>
+  </si>
+  <si>
+    <t>Brute force solved for 4 detectors.</t>
+  </si>
+  <si>
+    <t>Seems to follow noiseless solution</t>
+  </si>
+  <si>
+    <t>1dmockanderrors15</t>
+  </si>
+  <si>
+    <t>1dmockanderrors16</t>
   </si>
 </sst>
 </file>
@@ -285,8 +297,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M17" totalsRowShown="0">
-  <autoFilter ref="B3:M17" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M19" totalsRowShown="0">
+  <autoFilter ref="B3:M19" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
@@ -825,10 +837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:M17"/>
+  <dimension ref="B2:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,6 +1312,9 @@
       <c r="L14">
         <v>30</v>
       </c>
+      <c r="M14" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1335,6 +1350,9 @@
       <c r="L15">
         <v>30</v>
       </c>
+      <c r="M15" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1403,6 +1421,76 @@
         <v>10</v>
       </c>
       <c r="L17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18">
+        <v>200</v>
+      </c>
+      <c r="D18">
+        <v>200</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>1.5</v>
+      </c>
+      <c r="G18">
+        <v>60</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19">
+        <v>200</v>
+      </c>
+      <c r="D19">
+        <v>200</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>60</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed second brute force optimisation. added .py for brute force
</commit_message>
<xml_diff>
--- a/compressed_sensing/metadata.xlsx
+++ b/compressed_sensing/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{213011E1-DF3A-4728-9C14-03BF39FF574F}"/>
+  <xr:revisionPtr revIDLastSave="386" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1874BB4-1DE6-47A2-BB54-DEEEEBB881C5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -840,7 +840,7 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,7 +1389,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>51</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>54</v>
       </c>
@@ -1458,8 +1458,11 @@
       <c r="L18">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
finished 3rd brute force optimisation. Trying to draw conclutions.
</commit_message>
<xml_diff>
--- a/compressed_sensing/metadata.xlsx
+++ b/compressed_sensing/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="386" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1874BB4-1DE6-47A2-BB54-DEEEEBB881C5}"/>
+  <xr:revisionPtr revIDLastSave="405" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABB5EB79-459B-4376-83B9-D950F529FA46}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="2430" windowWidth="28725" windowHeight="10530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>1dmockanderrors16</t>
+  </si>
+  <si>
+    <t>training_set4</t>
+  </si>
+  <si>
+    <t>0.2-5</t>
   </si>
 </sst>
 </file>
@@ -839,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
   <dimension ref="B2:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,6 +1501,9 @@
       </c>
       <c r="L19">
         <v>30</v>
+      </c>
+      <c r="M19" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1510,13 +1519,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BFC62-FF4F-4DA1-97AB-A53A0749BD39}">
-  <dimension ref="B2:L6"/>
+  <dimension ref="B2:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -1661,6 +1679,38 @@
       </c>
       <c r="K6">
         <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+      <c r="D7">
+        <v>200</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7">
+        <v>60</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="J7">
+        <v>30</v>
+      </c>
+      <c r="K7">
+        <v>2500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>